<commit_message>
Enhance data with XLOOKUP for multiple rows, exact match and search order
</commit_message>
<xml_diff>
--- a/XLOOKUP.xlsx
+++ b/XLOOKUP.xlsx
@@ -8,12 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thonyalope\Documents\GitHub\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B063BA7-1D9F-47B6-894D-91D2BDB3DE99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D04F729E-E4C7-4C89-B01E-BEE753AF03BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="15585" xr2:uid="{5EA44D8F-79D3-45F5-A0F6-C7F47358B7ED}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="15585" activeTab="1" xr2:uid="{5EA44D8F-79D3-45F5-A0F6-C7F47358B7ED}"/>
   </bookViews>
   <sheets>
     <sheet name="XLOOKUP" sheetId="1" r:id="rId1"/>
+    <sheet name="XLOOKUP-MR" sheetId="2" r:id="rId2"/>
+    <sheet name="XLOOKUP-EM" sheetId="3" r:id="rId3"/>
+    <sheet name="XLOOKUP-SO" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,8 +36,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="48">
   <si>
     <t>EmployeeID</t>
   </si>
@@ -169,6 +194,15 @@
   </si>
   <si>
     <t>mchinchilla@gmail.com</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>Start Date</t>
+  </si>
+  <si>
+    <t>Person</t>
   </si>
 </sst>
 </file>
@@ -555,8 +589,8 @@
   </sheetPr>
   <dimension ref="A1:P23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1004,4 +1038,1396 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56D36371-336C-4855-B116-DE4EE7FD3DFD}">
+  <sheetPr>
+    <tabColor theme="4"/>
+  </sheetPr>
+  <dimension ref="A1:P10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.85546875" customWidth="1"/>
+    <col min="11" max="12" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="22.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="3" cm="1">
+        <f t="array" ref="B2:C2">_xlfn.XLOOKUP(A2,I2:I10,O2:P10)</f>
+        <v>42253</v>
+      </c>
+      <c r="C2" t="str">
+        <v>thonyalope@gmail.com</v>
+      </c>
+      <c r="F2" s="3">
+        <v>1001</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" s="3" t="str">
+        <f>CONCATENATE(G2," ", H2)</f>
+        <v>Anthony Vargas</v>
+      </c>
+      <c r="J2" s="3">
+        <v>27</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M2" s="3">
+        <v>45000</v>
+      </c>
+      <c r="N2" s="4">
+        <v>37197</v>
+      </c>
+      <c r="O2" s="4">
+        <v>42253</v>
+      </c>
+      <c r="P2" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="3" cm="1">
+        <f t="array" ref="B3:C3">_xlfn.XLOOKUP(A3,I3:I11,O3:P11)</f>
+        <v>42287</v>
+      </c>
+      <c r="C3" t="str">
+        <v>mvargas@gmail.com</v>
+      </c>
+      <c r="F3" s="3">
+        <v>1002</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" s="3" t="str">
+        <f t="shared" ref="I3:I10" si="0">CONCATENATE(G3," ", H3)</f>
+        <v>Manuel Vargas</v>
+      </c>
+      <c r="J3" s="3">
+        <v>52</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="M3" s="3">
+        <v>36000</v>
+      </c>
+      <c r="N3" s="4">
+        <v>36436</v>
+      </c>
+      <c r="O3" s="4">
+        <v>42287</v>
+      </c>
+      <c r="P3" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="3" cm="1">
+        <f t="array" ref="B4:C4">_xlfn.XLOOKUP(A4,I4:I12,O4:P12)</f>
+        <v>42986</v>
+      </c>
+      <c r="C4" t="str">
+        <v>nalvarado@gmail.com</v>
+      </c>
+      <c r="F4" s="3">
+        <v>1003</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>Norma Alvarado</v>
+      </c>
+      <c r="J4" s="3">
+        <v>50</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M4" s="3">
+        <v>63000</v>
+      </c>
+      <c r="N4" s="4">
+        <v>36711</v>
+      </c>
+      <c r="O4" s="4">
+        <v>42986</v>
+      </c>
+      <c r="P4" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="3" cm="1">
+        <f t="array" ref="B5:C5">_xlfn.XLOOKUP(A5,I5:I13,O5:P13)</f>
+        <v>42341</v>
+      </c>
+      <c r="C5" t="str">
+        <v>nvargas@gmail.com</v>
+      </c>
+      <c r="F5" s="3">
+        <v>1004</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>Ninoska Vargas</v>
+      </c>
+      <c r="J5" s="3">
+        <v>24</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M5" s="3">
+        <v>47000</v>
+      </c>
+      <c r="N5" s="4">
+        <v>36530</v>
+      </c>
+      <c r="O5" s="4">
+        <v>42341</v>
+      </c>
+      <c r="P5" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F6" s="3">
+        <v>1005</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I6" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>Josafat Vargas</v>
+      </c>
+      <c r="J6" s="3">
+        <v>25</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="M6" s="3">
+        <v>50000</v>
+      </c>
+      <c r="N6" s="4">
+        <v>37017</v>
+      </c>
+      <c r="O6" s="4">
+        <v>42977</v>
+      </c>
+      <c r="P6" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F7" s="3">
+        <v>1006</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I7" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>Victor Vargas</v>
+      </c>
+      <c r="J7" s="3">
+        <v>54</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="M7" s="3">
+        <v>65000</v>
+      </c>
+      <c r="N7" s="4">
+        <v>35040</v>
+      </c>
+      <c r="O7" s="4">
+        <v>41528</v>
+      </c>
+      <c r="P7" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F8" s="3">
+        <v>1007</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I8" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>Alejandro Rivera</v>
+      </c>
+      <c r="J8" s="3">
+        <v>29</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="M8" s="3">
+        <v>41000</v>
+      </c>
+      <c r="N8" s="4">
+        <v>37933</v>
+      </c>
+      <c r="O8" s="4">
+        <v>41551</v>
+      </c>
+      <c r="P8" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F9" s="3">
+        <v>1008</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I9" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>Anthony Castro</v>
+      </c>
+      <c r="J9" s="3">
+        <v>27</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M9" s="3">
+        <v>48000</v>
+      </c>
+      <c r="N9" s="4">
+        <v>37416</v>
+      </c>
+      <c r="O9" s="4">
+        <v>42116</v>
+      </c>
+      <c r="P9" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F10" s="3">
+        <v>1009</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I10" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>Marco Chinchilla</v>
+      </c>
+      <c r="J10" s="3">
+        <v>28</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M10" s="3">
+        <v>42000</v>
+      </c>
+      <c r="N10" s="4">
+        <v>37843</v>
+      </c>
+      <c r="O10" s="4">
+        <v>40800</v>
+      </c>
+      <c r="P10" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="P2" r:id="rId1" xr:uid="{C041AF95-825C-40CA-AA4A-DB7B546368CF}"/>
+    <hyperlink ref="P3:P10" r:id="rId2" display="thonyalope@gmail.com" xr:uid="{E07E5134-E26A-4837-BA33-269F22F497F0}"/>
+    <hyperlink ref="P3" r:id="rId3" xr:uid="{1DCAAA67-87E9-4CD2-85DA-D66F6390DABC}"/>
+    <hyperlink ref="P4" r:id="rId4" xr:uid="{9BEFBAFE-5C73-43E9-9E73-0B5CCD8182BB}"/>
+    <hyperlink ref="P5" r:id="rId5" xr:uid="{76279058-BC6A-45E3-9917-D96A3E2B787E}"/>
+    <hyperlink ref="P6" r:id="rId6" xr:uid="{34C3A269-CD2F-4CA8-826D-D1B0C43F3C37}"/>
+    <hyperlink ref="P7" r:id="rId7" xr:uid="{61196D30-C9C8-44AE-A27E-A86C0B2E12B5}"/>
+    <hyperlink ref="P8" r:id="rId8" xr:uid="{E51F9ABF-B955-478D-9EF7-2E0EED2DFEC8}"/>
+    <hyperlink ref="P9" r:id="rId9" xr:uid="{A81B17B3-3124-4348-9746-6114A18EA213}"/>
+    <hyperlink ref="P10" r:id="rId10" xr:uid="{BFADDF80-B855-4115-8F31-8EC34253F441}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C940D109-2F94-4B82-834B-A84CD9FD39A5}">
+  <sheetPr>
+    <tabColor theme="4"/>
+  </sheetPr>
+  <dimension ref="A1:O10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" customWidth="1"/>
+    <col min="8" max="8" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" customWidth="1"/>
+    <col min="11" max="11" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="22.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="3" t="str">
+        <f>_xlfn.XLOOKUP(A2,H2:H10,O2:O10,"Not Found")</f>
+        <v>thonyalope@gmail.com</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3">
+        <v>1001</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="3" t="str">
+        <f>CONCATENATE(F2," ", G2)</f>
+        <v>Anthony Vargas</v>
+      </c>
+      <c r="I2" s="3">
+        <v>27</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="3">
+        <v>45000</v>
+      </c>
+      <c r="M2" s="4">
+        <v>37197</v>
+      </c>
+      <c r="N2" s="4">
+        <v>42253</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="3" t="str">
+        <f t="shared" ref="B3:B5" si="0">_xlfn.XLOOKUP(A3,H3:H11,O3:O11,"Not Found")</f>
+        <v>mvargas@gmail.com</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3">
+        <v>1002</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="3" t="str">
+        <f t="shared" ref="H3:H10" si="1">CONCATENATE(F3," ", G3)</f>
+        <v>Manuel Vargas</v>
+      </c>
+      <c r="I3" s="3">
+        <v>52</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="L3" s="3">
+        <v>36000</v>
+      </c>
+      <c r="M3" s="4">
+        <v>36436</v>
+      </c>
+      <c r="N3" s="4">
+        <v>42287</v>
+      </c>
+      <c r="O3" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>nalvarado@gmail.com</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3">
+        <v>1003</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>Norma Alvarado</v>
+      </c>
+      <c r="I4" s="3">
+        <v>50</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="L4" s="3">
+        <v>63000</v>
+      </c>
+      <c r="M4" s="4">
+        <v>36711</v>
+      </c>
+      <c r="N4" s="4">
+        <v>42986</v>
+      </c>
+      <c r="O4" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>nvargas@gmail.com</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3">
+        <v>1004</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>Ninoska Vargas</v>
+      </c>
+      <c r="I5" s="3">
+        <v>24</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L5" s="3">
+        <v>47000</v>
+      </c>
+      <c r="M5" s="4">
+        <v>36530</v>
+      </c>
+      <c r="N5" s="4">
+        <v>42341</v>
+      </c>
+      <c r="O5" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3">
+        <v>1005</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>Josafat Vargas</v>
+      </c>
+      <c r="I6" s="3">
+        <v>25</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="L6" s="3">
+        <v>50000</v>
+      </c>
+      <c r="M6" s="4">
+        <v>37017</v>
+      </c>
+      <c r="N6" s="4">
+        <v>42977</v>
+      </c>
+      <c r="O6" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3">
+        <v>1006</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H7" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>Victor Vargas</v>
+      </c>
+      <c r="I7" s="3">
+        <v>54</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L7" s="3">
+        <v>65000</v>
+      </c>
+      <c r="M7" s="4">
+        <v>35040</v>
+      </c>
+      <c r="N7" s="4">
+        <v>41528</v>
+      </c>
+      <c r="O7" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3">
+        <v>1007</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H8" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>Alejandro Rivera</v>
+      </c>
+      <c r="I8" s="3">
+        <v>29</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="L8" s="3">
+        <v>41000</v>
+      </c>
+      <c r="M8" s="4">
+        <v>37933</v>
+      </c>
+      <c r="N8" s="4">
+        <v>41551</v>
+      </c>
+      <c r="O8" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3">
+        <v>1008</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H9" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>Anthony Castro</v>
+      </c>
+      <c r="I9" s="3">
+        <v>27</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="L9" s="3">
+        <v>48000</v>
+      </c>
+      <c r="M9" s="4">
+        <v>37416</v>
+      </c>
+      <c r="N9" s="4">
+        <v>42116</v>
+      </c>
+      <c r="O9" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3">
+        <v>1009</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H10" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>Marco Chinchilla</v>
+      </c>
+      <c r="I10" s="3">
+        <v>28</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L10" s="3">
+        <v>42000</v>
+      </c>
+      <c r="M10" s="4">
+        <v>37843</v>
+      </c>
+      <c r="N10" s="4">
+        <v>40800</v>
+      </c>
+      <c r="O10" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="O2" r:id="rId1" xr:uid="{BDC17127-28D1-4202-9978-FD9149BED9A0}"/>
+    <hyperlink ref="O3:O10" r:id="rId2" display="thonyalope@gmail.com" xr:uid="{97E60276-5D50-40A0-A50C-D37563B7D01F}"/>
+    <hyperlink ref="O3" r:id="rId3" xr:uid="{DD99356D-A1E9-4526-B0A6-9F6E4C499F3C}"/>
+    <hyperlink ref="O4" r:id="rId4" xr:uid="{0191B4A6-05BA-44A5-8364-3663DCDE01F4}"/>
+    <hyperlink ref="O5" r:id="rId5" xr:uid="{88E244C4-9430-4C03-A4DD-F69DB631EE2A}"/>
+    <hyperlink ref="O6" r:id="rId6" xr:uid="{1B64BC68-4079-45F3-B90B-A3B397C6C4C5}"/>
+    <hyperlink ref="O7" r:id="rId7" xr:uid="{C82DF6A0-064B-482D-A2FD-8A904AA362FC}"/>
+    <hyperlink ref="O8" r:id="rId8" xr:uid="{80199B9D-53D1-45CA-A892-2DD7D4A37C88}"/>
+    <hyperlink ref="O9" r:id="rId9" xr:uid="{A6E54DB5-6DD6-4E50-ACE6-DAC5379C25B7}"/>
+    <hyperlink ref="O10" r:id="rId10" xr:uid="{69F26B6E-B792-4651-BB9B-CB176D448BB2}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80B1DD7A-85E3-4D23-BE4F-B3091AD44488}">
+  <sheetPr>
+    <tabColor theme="4"/>
+  </sheetPr>
+  <dimension ref="A1:P10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K30" sqref="K30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.85546875" customWidth="1"/>
+    <col min="12" max="12" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="11" customWidth="1"/>
+    <col min="16" max="16" width="27.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>36711</v>
+      </c>
+      <c r="B2" s="3" t="str">
+        <f>_xlfn.XLOOKUP(A2,N2:N10,I2:I10,,1)</f>
+        <v>Norma Alvarado</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3">
+        <v>1001</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" s="3" t="str">
+        <f>CONCATENATE(G2," ", H2)</f>
+        <v>Anthony Vargas</v>
+      </c>
+      <c r="J2" s="3">
+        <v>27</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M2" s="3">
+        <v>45000</v>
+      </c>
+      <c r="N2" s="4">
+        <v>37197</v>
+      </c>
+      <c r="O2" s="4">
+        <v>42253</v>
+      </c>
+      <c r="P2" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>35040</v>
+      </c>
+      <c r="B3" s="3" t="str">
+        <f t="shared" ref="B3:B5" si="0">_xlfn.XLOOKUP(A3,N3:N11,I3:I11,,1)</f>
+        <v>Victor Vargas</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3">
+        <v>1002</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" s="3" t="str">
+        <f t="shared" ref="I3:I10" si="1">CONCATENATE(G3," ", H3)</f>
+        <v>Manuel Vargas</v>
+      </c>
+      <c r="J3" s="3">
+        <v>52</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="M3" s="3">
+        <v>36000</v>
+      </c>
+      <c r="N3" s="4">
+        <v>36436</v>
+      </c>
+      <c r="O3" s="4">
+        <v>42287</v>
+      </c>
+      <c r="P3" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>37416</v>
+      </c>
+      <c r="B4" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>Anthony Castro</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3">
+        <v>1003</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>Norma Alvarado</v>
+      </c>
+      <c r="J4" s="3">
+        <v>50</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M4" s="3">
+        <v>63000</v>
+      </c>
+      <c r="N4" s="4">
+        <v>36711</v>
+      </c>
+      <c r="O4" s="4">
+        <v>42986</v>
+      </c>
+      <c r="P4" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>37197</v>
+      </c>
+      <c r="B5" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>Anthony Castro</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3">
+        <v>1004</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>Ninoska Vargas</v>
+      </c>
+      <c r="J5" s="3">
+        <v>24</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M5" s="3">
+        <v>47000</v>
+      </c>
+      <c r="N5" s="4">
+        <v>36530</v>
+      </c>
+      <c r="O5" s="4">
+        <v>42341</v>
+      </c>
+      <c r="P5" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3">
+        <v>1005</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I6" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>Josafat Vargas</v>
+      </c>
+      <c r="J6" s="3">
+        <v>25</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="M6" s="3">
+        <v>50000</v>
+      </c>
+      <c r="N6" s="4">
+        <v>37017</v>
+      </c>
+      <c r="O6" s="4">
+        <v>42977</v>
+      </c>
+      <c r="P6" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3">
+        <v>1006</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I7" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>Victor Vargas</v>
+      </c>
+      <c r="J7" s="3">
+        <v>54</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="M7" s="3">
+        <v>65000</v>
+      </c>
+      <c r="N7" s="4">
+        <v>35040</v>
+      </c>
+      <c r="O7" s="4">
+        <v>41528</v>
+      </c>
+      <c r="P7" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3">
+        <v>1007</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I8" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>Alejandro Rivera</v>
+      </c>
+      <c r="J8" s="3">
+        <v>29</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="M8" s="3">
+        <v>41000</v>
+      </c>
+      <c r="N8" s="4">
+        <v>37933</v>
+      </c>
+      <c r="O8" s="4">
+        <v>41551</v>
+      </c>
+      <c r="P8" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3">
+        <v>1008</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I9" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>Anthony Castro</v>
+      </c>
+      <c r="J9" s="3">
+        <v>27</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M9" s="3">
+        <v>48000</v>
+      </c>
+      <c r="N9" s="4">
+        <v>37416</v>
+      </c>
+      <c r="O9" s="4">
+        <v>42116</v>
+      </c>
+      <c r="P9" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3">
+        <v>1009</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I10" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>Marco Chinchilla</v>
+      </c>
+      <c r="J10" s="3">
+        <v>28</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M10" s="3">
+        <v>42000</v>
+      </c>
+      <c r="N10" s="4">
+        <v>37843</v>
+      </c>
+      <c r="O10" s="4">
+        <v>40800</v>
+      </c>
+      <c r="P10" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="P2" r:id="rId1" xr:uid="{534D22FC-3F64-4F66-94A1-266C1C3E6945}"/>
+    <hyperlink ref="P3:P10" r:id="rId2" display="thonyalope@gmail.com" xr:uid="{38AB19B1-2B6D-428D-A2CA-1ECB1C9681BF}"/>
+    <hyperlink ref="P3" r:id="rId3" xr:uid="{34447B80-FDEA-47AF-8AB0-E8714EBE9082}"/>
+    <hyperlink ref="P4" r:id="rId4" xr:uid="{236AA1D7-BBC1-463C-B98E-22D4C350A612}"/>
+    <hyperlink ref="P5" r:id="rId5" xr:uid="{611C2870-E932-4D16-ACA8-1D6B7396818C}"/>
+    <hyperlink ref="P6" r:id="rId6" xr:uid="{3343519F-7303-41C2-B5F2-9C0155D2FDF4}"/>
+    <hyperlink ref="P7" r:id="rId7" xr:uid="{9D52A5AC-EAAD-4206-8F42-4D9030779EC8}"/>
+    <hyperlink ref="P8" r:id="rId8" xr:uid="{567C9821-B2A0-4D26-82A9-F2F7E5755B78}"/>
+    <hyperlink ref="P9" r:id="rId9" xr:uid="{0AE47C04-AB60-48A1-B661-5587D54EE15D}"/>
+    <hyperlink ref="P10" r:id="rId10" xr:uid="{8638C55B-89D8-423E-84B1-1ED3C3928076}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>